<commit_message>
Updated grade helper spreadsheet.
</commit_message>
<xml_diff>
--- a/grade_helper.xlsx
+++ b/grade_helper.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarahm\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885BE6DA-9F90-4659-A3B6-BF2926D55C17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B1C115-F1BB-4E79-9C59-2889DA5FA729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6720" xr2:uid="{B5911BD4-29A2-47B5-BC24-1FB3953DE2CE}"/>
+    <workbookView xWindow="28680" yWindow="-3615" windowWidth="29040" windowHeight="15720" xr2:uid="{B5911BD4-29A2-47B5-BC24-1FB3953DE2CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Predict and Enter!</t>
   </si>
@@ -64,13 +75,31 @@
   </si>
   <si>
     <t>Note: If you plan to take the optional final, replace your lowest exam score with what you expect to get on the final (out of 150 pts)</t>
+  </si>
+  <si>
+    <t>When guessing your final project %:</t>
+  </si>
+  <si>
+    <t>Middle C = 75%</t>
+  </si>
+  <si>
+    <t>Middle B = 85%</t>
+  </si>
+  <si>
+    <t>Middle A = 95%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(To get above 95%, you'll want to go a little above and beyond the specifications, like making your python front end have a </t>
+  </si>
+  <si>
+    <t>main function/menu system and/or do a really good job on comments in your queries and program.)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,13 +125,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -155,12 +177,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -181,9 +202,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -221,7 +242,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -327,7 +348,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -469,7 +490,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -477,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08203F40-C660-4F0A-9831-1FBA10B9C8F7}">
-  <dimension ref="B1:J6"/>
+  <dimension ref="B1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.109375" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -505,7 +526,7 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
@@ -562,7 +583,7 @@
       <c r="F3" s="2">
         <v>0</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="2">
         <v>0</v>
       </c>
       <c r="H3">
@@ -580,6 +601,36 @@
     <row r="6" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>